<commit_message>
upload code for analysis
</commit_message>
<xml_diff>
--- a/Employee_Survey_Results.xlsx
+++ b/Employee_Survey_Results.xlsx
@@ -1,25 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabed1\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3685F57C-F966-4AC6-9D88-F1C6A7C69C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6627E370-05B0-4FC0-A403-E177FB9F9621}"/>
+    <workbookView windowWidth="24750" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -27,6 +18,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -63,25 +56,368 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -89,9 +425,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -102,17 +680,61 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -161,7 +783,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -194,26 +816,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -246,23 +851,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -404,34 +992,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2AB851C-E75D-43EB-BEED-4A9B5D74B16A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5583333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.2166666666667" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.4416666666667" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.2166666666667" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.1083333333333" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +1034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -471,7 +1054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -491,7 +1074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -511,7 +1094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -531,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -551,7 +1134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -571,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -591,7 +1174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -611,7 +1194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -631,7 +1214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -651,7 +1234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -671,7 +1254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -691,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -711,7 +1294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -731,7 +1314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -751,7 +1334,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -771,7 +1354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -791,7 +1374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -811,7 +1394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -831,7 +1414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -851,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -871,7 +1454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -891,7 +1474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -911,7 +1494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -931,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -951,7 +1534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -971,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -991,7 +1574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1011,7 +1594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1031,7 +1614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1051,7 +1634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1071,7 +1654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1091,7 +1674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1111,7 +1694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1131,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1151,7 +1734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1171,7 +1754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1191,7 +1774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1211,7 +1794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1231,7 +1814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1251,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1271,7 +1854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1291,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1311,7 +1894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1331,7 +1914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1351,7 +1934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1371,7 +1954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1391,7 +1974,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1411,7 +1994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1431,7 +2014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1453,5 +2036,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>